<commit_message>
fix: Correção na Coluna B - 2024 - arquivo anual
</commit_message>
<xml_diff>
--- a/data/processed/Anual/2024/2024.xlsx
+++ b/data/processed/Anual/2024/2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="26">
   <si>
     <t xml:space="preserve">Estado</t>
   </si>
@@ -110,7 +110,7 @@
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +132,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,7 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -198,6 +204,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,8 +402,8 @@
   </sheetPr>
   <dimension ref="A1:J649"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A174" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.66796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1315,7 +1325,6 @@
       <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="0"/>
       <c r="D30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1527,8 +1536,8 @@
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="1" t="n">
-        <v>5</v>
+      <c r="B37" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>6</v>

</xml_diff>